<commit_message>
added execption handling to get around tweepy errors
</commit_message>
<xml_diff>
--- a/improvement data.xlsx
+++ b/improvement data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Known bot spotters" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Aek_bot</t>
-  </si>
-  <si>
-    <t>check first</t>
   </si>
   <si>
     <t>error</t>
@@ -433,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +441,7 @@
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -460,7 +457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -468,7 +465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -476,7 +473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -484,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -492,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -500,15 +497,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -539,27 +533,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -571,13 +565,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to do responsible exception handling
</commit_message>
<xml_diff>
--- a/improvement data.xlsx
+++ b/improvement data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Known bot spotters" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>